<commit_message>
25% faster if function is used
</commit_message>
<xml_diff>
--- a/python/python_vs_c.xlsx
+++ b/python/python_vs_c.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Library\github\prime\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523F5A2F-1270-400B-9AFF-752FB96C01B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F96DDED-290B-4157-B8D3-6BD2A7512873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10080" yWindow="615" windowWidth="22755" windowHeight="15030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30825" yWindow="6045" windowWidth="22755" windowHeight="15030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2023" sheetId="2" r:id="rId1"/>
+    <sheet name="2022" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
   <si>
     <t>Python</t>
   </si>
@@ -95,6 +96,18 @@
   </si>
   <si>
     <t xml:space="preserve">https://github.com/kreier/prime/tree/main/arduino </t>
+  </si>
+  <si>
+    <t>rp2040 133 MHz</t>
+  </si>
+  <si>
+    <t>CircuitPython 8.2.8</t>
+  </si>
+  <si>
+    <t>i3 4100 MHz</t>
+  </si>
+  <si>
+    <t>code v3.0</t>
   </si>
 </sst>
 </file>
@@ -106,7 +119,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -180,6 +193,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -260,12 +280,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -481,20 +501,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53583A92-6E91-471D-AE71-015DF5BF3E3A}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" customWidth="1"/>
     <col min="4" max="9" width="8.85546875" customWidth="1"/>
     <col min="10" max="12" width="8.85546875" style="18" customWidth="1"/>
@@ -533,7 +553,7 @@
         <v>3200</v>
       </c>
       <c r="L1" s="15">
-        <v>3600</v>
+        <v>4100</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -576,120 +596,636 @@
       <c r="A3" s="4">
         <v>1000</v>
       </c>
-      <c r="B3" s="2">
-        <v>168</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0.69399999999999995</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0.182</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0.11</v>
-      </c>
-      <c r="F3" s="5">
-        <v>3.5999999999999997E-2</v>
-      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
       <c r="G3" s="5">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="H3" s="5">
-        <v>0.13900000000000001</v>
-      </c>
-      <c r="I3" s="5">
-        <v>2.7E-2</v>
-      </c>
-      <c r="J3" s="17">
-        <v>1.6E-2</v>
-      </c>
-      <c r="K3" s="17">
-        <v>0</v>
-      </c>
-      <c r="L3" s="25">
-        <v>0</v>
+        <v>3.7789999999999997E-2</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="24">
+        <v>3.7389999999999998E-4</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>10000</v>
       </c>
-      <c r="B4" s="2">
-        <v>1.2290000000000001</v>
-      </c>
-      <c r="C4" s="5">
-        <v>13.516999999999999</v>
-      </c>
-      <c r="D4" s="5">
-        <v>3.36</v>
-      </c>
-      <c r="E4" s="5">
-        <v>1.97</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0.626</v>
-      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
       <c r="G4" s="5">
-        <v>0.79700000000000004</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0.76900000000000002</v>
-      </c>
-      <c r="I4" s="5">
-        <v>0.48699999999999999</v>
-      </c>
-      <c r="J4" s="17">
-        <v>0.25900000000000001</v>
-      </c>
-      <c r="K4" s="17">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="L4" s="25">
-        <v>0</v>
+        <v>0.94677699999999998</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="24">
+        <v>5.2383000000000004E-3</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>100000</v>
       </c>
-      <c r="B5" s="2">
-        <v>9.5920000000000005</v>
-      </c>
-      <c r="C5" s="5">
-        <v>318.459</v>
-      </c>
-      <c r="D5" s="5">
-        <v>71.007999999999996</v>
-      </c>
-      <c r="E5" s="5">
-        <v>40.950000000000003</v>
-      </c>
-      <c r="F5" s="5">
-        <v>12.766</v>
-      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
       <c r="G5" s="5">
-        <v>17.027999999999999</v>
-      </c>
-      <c r="H5" s="5">
-        <v>10.278</v>
-      </c>
-      <c r="I5" s="5">
-        <v>10.037000000000001</v>
-      </c>
-      <c r="J5" s="17">
-        <v>5.6070000000000002</v>
-      </c>
-      <c r="K5" s="17">
-        <v>0.111</v>
-      </c>
-      <c r="L5" s="26">
-        <v>0.1089</v>
+        <v>12.3901</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="25">
+        <v>9.1182083999999997E-2</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>1000000</v>
       </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5">
+        <v>384.29599999999999</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="25">
+        <v>1.4816269</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="25">
+        <v>57.317262640000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="26"/>
+      <c r="G8" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>1000</v>
+      </c>
+      <c r="B12" s="12">
+        <v>168</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="15"/>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>10000</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1229</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="15"/>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>100000</v>
+      </c>
+      <c r="B14" s="4">
+        <v>9592</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="18">
+        <v>6.0790000000000002E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>1000000</v>
+      </c>
+      <c r="B15" s="4">
+        <v>78498</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="18">
+        <v>0.125029</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L16" s="18">
+        <v>3.0749499999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18" s="13" t="e">
+        <f>D3/D12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E18" s="13" t="e">
+        <f>E3/E12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F18" s="13" t="e">
+        <f>F3/F12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G18" s="13" t="e">
+        <f>G3/G12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H18" s="13" t="e">
+        <f>H3/H12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I18" s="13" t="e">
+        <f>I3/I12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J18" s="22" t="e">
+        <f>J3/J12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K18" s="22" t="e">
+        <f>K3/K12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L18" s="22" t="e">
+        <f t="shared" ref="L18" si="0">L3/L12</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="13" t="e">
+        <f>D4/D13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E19" s="13" t="e">
+        <f>E4/E13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F19" s="13" t="e">
+        <f>F4/F13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G19" s="13" t="e">
+        <f>G4/G13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H19" s="13" t="e">
+        <f>H4/H13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I19" s="13" t="e">
+        <f>I4/I13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J19" s="22" t="e">
+        <f>J4/J13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K19" s="22" t="e">
+        <f>K4/K13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L19" s="22" t="e">
+        <f t="shared" ref="L19" si="1">L4/L13</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="13" t="e">
+        <f>D5/D14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E20" s="13" t="e">
+        <f>E5/E14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F20" s="13" t="e">
+        <f>F5/F14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G20" s="13" t="e">
+        <f>G5/G14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H20" s="13" t="e">
+        <f>H5/H14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I20" s="13" t="e">
+        <f>I5/I14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J20" s="22" t="e">
+        <f>J5/J14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K20" s="22" t="e">
+        <f>K5/K14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L20" s="22">
+        <f t="shared" ref="L20" si="2">L5/L14</f>
+        <v>14.999520315841421</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="13" t="e">
+        <f>D6/D15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E21" s="13" t="e">
+        <f>E6/E15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F21" s="13" t="e">
+        <f>F6/F15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G21" s="13" t="e">
+        <f>G6/G15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H21" s="13" t="e">
+        <f>H6/H15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I21" s="13" t="e">
+        <f>I6/I15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J21" s="22" t="e">
+        <f>J6/J15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K21" s="22" t="e">
+        <f>K6/K15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L21" s="22">
+        <f t="shared" ref="L21:L22" si="3">L6/L15</f>
+        <v>11.850265938302314</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="22">
+        <f t="shared" si="3"/>
+        <v>18.640063298590224</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C10" r:id="rId1" xr:uid="{D8C2202D-C06C-4E48-8367-22B62D35A86B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:L21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="4" max="9" width="8.85546875" customWidth="1"/>
+    <col min="10" max="12" width="8.85546875" style="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2">
+        <v>80</v>
+      </c>
+      <c r="E1" s="2">
+        <v>160</v>
+      </c>
+      <c r="F1" s="2">
+        <v>240</v>
+      </c>
+      <c r="G1" s="2">
+        <v>125</v>
+      </c>
+      <c r="H1" s="2">
+        <v>240</v>
+      </c>
+      <c r="I1" s="2">
+        <v>160</v>
+      </c>
+      <c r="J1" s="15">
+        <v>240</v>
+      </c>
+      <c r="K1" s="15">
+        <v>3200</v>
+      </c>
+      <c r="L1" s="15">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>1000</v>
+      </c>
+      <c r="B3" s="2">
+        <v>168</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.182</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0.11</v>
+      </c>
+      <c r="F3" s="5">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="G3" s="5">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="I3" s="5">
+        <v>2.7E-2</v>
+      </c>
+      <c r="J3" s="17">
+        <v>1.6E-2</v>
+      </c>
+      <c r="K3" s="17">
+        <v>0</v>
+      </c>
+      <c r="L3" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>10000</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.2290000000000001</v>
+      </c>
+      <c r="C4" s="5">
+        <v>13.516999999999999</v>
+      </c>
+      <c r="D4" s="5">
+        <v>3.36</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1.97</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.626</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="J4" s="17">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="K4" s="17">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="L4" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>100000</v>
+      </c>
+      <c r="B5" s="2">
+        <v>9.5920000000000005</v>
+      </c>
+      <c r="C5" s="5">
+        <v>318.459</v>
+      </c>
+      <c r="D5" s="5">
+        <v>71.007999999999996</v>
+      </c>
+      <c r="E5" s="5">
+        <v>40.950000000000003</v>
+      </c>
+      <c r="F5" s="5">
+        <v>12.766</v>
+      </c>
+      <c r="G5" s="5">
+        <v>17.027999999999999</v>
+      </c>
+      <c r="H5" s="5">
+        <v>10.278</v>
+      </c>
+      <c r="I5" s="5">
+        <v>10.037000000000001</v>
+      </c>
+      <c r="J5" s="17">
+        <v>5.6070000000000002</v>
+      </c>
+      <c r="K5" s="17">
+        <v>0.111</v>
+      </c>
+      <c r="L5" s="25">
+        <v>0.1089</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>1000000</v>
+      </c>
       <c r="B6" s="2">
         <v>78.498000000000005</v>
       </c>
@@ -716,7 +1252,7 @@
       <c r="K6" s="17">
         <v>2.5990000000000002</v>
       </c>
-      <c r="L6" s="26">
+      <c r="L6" s="25">
         <v>2.4839000000000002</v>
       </c>
     </row>
@@ -727,17 +1263,13 @@
       <c r="B9" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>12</v>
       </c>
@@ -755,7 +1287,7 @@
         <v>16</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="H10" s="19" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
comparisons in 2023 with new Circuitpython
</commit_message>
<xml_diff>
--- a/python/python_vs_c.xlsx
+++ b/python/python_vs_c.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Library\github\prime\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F96DDED-290B-4157-B8D3-6BD2A7512873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5930FFA-5EF5-4235-8122-C63EF5DF986D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30825" yWindow="6045" windowWidth="22755" windowHeight="15030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33255" yWindow="2175" windowWidth="15705" windowHeight="13245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
   <si>
     <t>Python</t>
   </si>
@@ -108,16 +108,29 @@
   </si>
   <si>
     <t>code v3.0</t>
+  </si>
+  <si>
+    <t>prime to</t>
+  </si>
+  <si>
+    <t>factor</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="172" formatCode="0.00000"/>
+    <numFmt numFmtId="173" formatCode="0.000000"/>
+    <numFmt numFmtId="175" formatCode="0.000"/>
+    <numFmt numFmtId="176" formatCode="#,##0.00000"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -201,12 +214,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -222,7 +241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -286,6 +305,25 @@
     </xf>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="175" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -505,10 +543,569 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="3" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="9" width="8.85546875" style="18" customWidth="1"/>
+    <col min="10" max="10" width="2.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>240</v>
+      </c>
+      <c r="D1" s="2">
+        <v>125</v>
+      </c>
+      <c r="E1" s="2">
+        <v>240</v>
+      </c>
+      <c r="F1" s="2">
+        <v>160</v>
+      </c>
+      <c r="G1" s="15">
+        <v>240</v>
+      </c>
+      <c r="H1" s="15">
+        <v>3200</v>
+      </c>
+      <c r="I1" s="15">
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>1000</v>
+      </c>
+      <c r="B3" s="12">
+        <v>168</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.106934</v>
+      </c>
+      <c r="D3" s="5">
+        <v>3.60107E-2</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0.109985</v>
+      </c>
+      <c r="F3" s="31"/>
+      <c r="G3" s="17">
+        <v>1.49994E-2</v>
+      </c>
+      <c r="H3" s="30">
+        <v>1.7432999999999999E-4</v>
+      </c>
+      <c r="I3" s="30">
+        <v>2.8400000000000002E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>10000</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1229</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2.2850000000000001</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.58398399999999995</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.515015</v>
+      </c>
+      <c r="F4" s="31"/>
+      <c r="G4" s="17">
+        <v>0.235016</v>
+      </c>
+      <c r="H4" s="17">
+        <v>2.1991249950000001E-3</v>
+      </c>
+      <c r="I4" s="24">
+        <v>3.8470000000000002E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>100000</v>
+      </c>
+      <c r="B5" s="4">
+        <v>9592</v>
+      </c>
+      <c r="C5" s="5">
+        <v>54.3979</v>
+      </c>
+      <c r="D5" s="5">
+        <v>11.536</v>
+      </c>
+      <c r="E5" s="5">
+        <v>8.5470000000000006</v>
+      </c>
+      <c r="F5" s="31"/>
+      <c r="G5" s="17">
+        <v>4.6789990000000001</v>
+      </c>
+      <c r="H5" s="17">
+        <v>3.568429E-2</v>
+      </c>
+      <c r="I5" s="25">
+        <v>6.7795999999999995E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>1000000</v>
+      </c>
+      <c r="B6" s="4">
+        <v>78498</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1356.84</v>
+      </c>
+      <c r="D6" s="5">
+        <v>261.43799999999999</v>
+      </c>
+      <c r="E6" s="5">
+        <v>169.59100000000001</v>
+      </c>
+      <c r="F6" s="31"/>
+      <c r="G6" s="17">
+        <v>106.679</v>
+      </c>
+      <c r="H6" s="17">
+        <v>0.96153670000000002</v>
+      </c>
+      <c r="I6" s="25">
+        <v>1.4816269</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17">
+        <v>24.750426000000001</v>
+      </c>
+      <c r="I7" s="25">
+        <v>57.317262640000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="L11" s="34">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>1000</v>
+      </c>
+      <c r="B12" s="12">
+        <v>168</v>
+      </c>
+      <c r="C12" s="29">
+        <v>0.01</v>
+      </c>
+      <c r="D12" s="29">
+        <v>0.01</v>
+      </c>
+      <c r="E12" s="31"/>
+      <c r="F12" s="29">
+        <v>0.02</v>
+      </c>
+      <c r="G12" s="29">
+        <v>0.01</v>
+      </c>
+      <c r="H12" s="27">
+        <v>3.1999999999999999E-5</v>
+      </c>
+      <c r="I12" s="28">
+        <v>1.9000000000000001E-5</v>
+      </c>
+      <c r="K12" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="L12" s="5">
+        <v>599.49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>10000</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1229</v>
+      </c>
+      <c r="C13" s="29">
+        <v>0.24</v>
+      </c>
+      <c r="D13" s="29">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E13" s="31"/>
+      <c r="F13" s="29">
+        <v>0.43</v>
+      </c>
+      <c r="G13" s="29">
+        <v>0.22</v>
+      </c>
+      <c r="H13" s="27">
+        <v>2.33E-4</v>
+      </c>
+      <c r="I13" s="28">
+        <v>2.9700000000000001E-4</v>
+      </c>
+      <c r="K13" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="L13" s="29">
+        <v>8.6038000000000003E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>100000</v>
+      </c>
+      <c r="B14" s="4">
+        <v>9592</v>
+      </c>
+      <c r="C14" s="29">
+        <v>5.67</v>
+      </c>
+      <c r="D14" s="29">
+        <v>3.29</v>
+      </c>
+      <c r="E14" s="31"/>
+      <c r="F14" s="29">
+        <v>10.16</v>
+      </c>
+      <c r="G14" s="29">
+        <v>5.22</v>
+      </c>
+      <c r="H14" s="27">
+        <v>6.7099999999999998E-3</v>
+      </c>
+      <c r="I14" s="28">
+        <v>6.0790000000000002E-3</v>
+      </c>
+      <c r="K14" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="L14" s="35">
+        <f>L12/L13</f>
+        <v>6967.7351867779353</v>
+      </c>
+      <c r="M14" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>1000000</v>
+      </c>
+      <c r="B15" s="4">
+        <v>78498</v>
+      </c>
+      <c r="C15" s="29">
+        <v>141.02000000000001</v>
+      </c>
+      <c r="D15" s="29">
+        <v>82.03</v>
+      </c>
+      <c r="E15" s="31"/>
+      <c r="F15" s="29">
+        <v>252.73</v>
+      </c>
+      <c r="G15" s="29">
+        <v>129.94999999999999</v>
+      </c>
+      <c r="H15" s="27">
+        <v>8.6038000000000003E-2</v>
+      </c>
+      <c r="I15" s="28">
+        <v>0.125029</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="27">
+        <v>1.1831149999999999</v>
+      </c>
+      <c r="I16" s="28">
+        <v>3.0749499999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18" s="13">
+        <f t="shared" ref="C18:H21" si="0">C3/C12</f>
+        <v>10.6934</v>
+      </c>
+      <c r="D18" s="13">
+        <f t="shared" si="0"/>
+        <v>3.60107</v>
+      </c>
+      <c r="E18" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F18" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="22">
+        <f t="shared" si="0"/>
+        <v>1.4999399999999998</v>
+      </c>
+      <c r="H18" s="22">
+        <f t="shared" si="0"/>
+        <v>5.4478125000000004</v>
+      </c>
+      <c r="I18" s="22">
+        <f t="shared" ref="I18" si="1">I3/I12</f>
+        <v>14.947368421052632</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19" s="13">
+        <f t="shared" si="0"/>
+        <v>9.5208333333333339</v>
+      </c>
+      <c r="D19" s="13">
+        <f t="shared" si="0"/>
+        <v>4.1713142857142849</v>
+      </c>
+      <c r="E19" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F19" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="22">
+        <f t="shared" si="0"/>
+        <v>1.0682545454545456</v>
+      </c>
+      <c r="H19" s="22">
+        <f t="shared" si="0"/>
+        <v>9.438304699570816</v>
+      </c>
+      <c r="I19" s="22">
+        <f t="shared" ref="I19" si="2">I4/I13</f>
+        <v>12.952861952861953</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20" s="13">
+        <f t="shared" si="0"/>
+        <v>9.5939858906525579</v>
+      </c>
+      <c r="D20" s="13">
+        <f t="shared" si="0"/>
+        <v>3.506382978723404</v>
+      </c>
+      <c r="E20" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F20" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="22">
+        <f t="shared" si="0"/>
+        <v>0.89635996168582377</v>
+      </c>
+      <c r="H20" s="22">
+        <f t="shared" si="0"/>
+        <v>5.3180760059612524</v>
+      </c>
+      <c r="I20" s="22">
+        <f t="shared" ref="I20" si="3">I5/I14</f>
+        <v>11.152492186214836</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21" s="13">
+        <f t="shared" si="0"/>
+        <v>9.6216139554673088</v>
+      </c>
+      <c r="D21" s="13">
+        <f t="shared" si="0"/>
+        <v>3.1871022796537849</v>
+      </c>
+      <c r="E21" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F21" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="22">
+        <f t="shared" si="0"/>
+        <v>0.82092343208926521</v>
+      </c>
+      <c r="H21" s="22">
+        <f t="shared" si="0"/>
+        <v>11.17572119296125</v>
+      </c>
+      <c r="I21" s="22">
+        <f t="shared" ref="H21:I22" si="4">I6/I15</f>
+        <v>11.850265938302314</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="22">
+        <f t="shared" si="4"/>
+        <v>20.919712792078542</v>
+      </c>
+      <c r="I22" s="22">
+        <f t="shared" si="4"/>
+        <v>18.640063298590224</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C10" r:id="rId1" xr:uid="{D8C2202D-C06C-4E48-8367-22B62D35A86B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:L21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -553,522 +1150,6 @@
         <v>3200</v>
       </c>
       <c r="L1" s="15">
-        <v>4100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>1000</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5">
-        <v>3.7789999999999997E-2</v>
-      </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="24">
-        <v>3.7389999999999998E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>10000</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5">
-        <v>0.94677699999999998</v>
-      </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="24">
-        <v>5.2383000000000004E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>100000</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5">
-        <v>12.3901</v>
-      </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="25">
-        <v>9.1182083999999997E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>1000000</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5">
-        <v>384.29599999999999</v>
-      </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="25">
-        <v>1.4816269</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>10000000</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="25">
-        <v>57.317262640000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="26"/>
-      <c r="G8" s="26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="J11" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="K11" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L11" s="19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>1000</v>
-      </c>
-      <c r="B12" s="12">
-        <v>168</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="15"/>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>10000</v>
-      </c>
-      <c r="B13" s="4">
-        <v>1229</v>
-      </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="15"/>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>100000</v>
-      </c>
-      <c r="B14" s="4">
-        <v>9592</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="18">
-        <v>6.0790000000000002E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>1000000</v>
-      </c>
-      <c r="B15" s="4">
-        <v>78498</v>
-      </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="18">
-        <v>0.125029</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L16" s="18">
-        <v>3.0749499999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18" s="13" t="e">
-        <f>D3/D12</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E18" s="13" t="e">
-        <f>E3/E12</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F18" s="13" t="e">
-        <f>F3/F12</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G18" s="13" t="e">
-        <f>G3/G12</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H18" s="13" t="e">
-        <f>H3/H12</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I18" s="13" t="e">
-        <f>I3/I12</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J18" s="22" t="e">
-        <f>J3/J12</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K18" s="22" t="e">
-        <f>K3/K12</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L18" s="22" t="e">
-        <f t="shared" ref="L18" si="0">L3/L12</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="13" t="e">
-        <f>D4/D13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E19" s="13" t="e">
-        <f>E4/E13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F19" s="13" t="e">
-        <f>F4/F13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G19" s="13" t="e">
-        <f>G4/G13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H19" s="13" t="e">
-        <f>H4/H13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I19" s="13" t="e">
-        <f>I4/I13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J19" s="22" t="e">
-        <f>J4/J13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K19" s="22" t="e">
-        <f>K4/K13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L19" s="22" t="e">
-        <f t="shared" ref="L19" si="1">L4/L13</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="13" t="e">
-        <f>D5/D14</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E20" s="13" t="e">
-        <f>E5/E14</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F20" s="13" t="e">
-        <f>F5/F14</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G20" s="13" t="e">
-        <f>G5/G14</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H20" s="13" t="e">
-        <f>H5/H14</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I20" s="13" t="e">
-        <f>I5/I14</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J20" s="22" t="e">
-        <f>J5/J14</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K20" s="22" t="e">
-        <f>K5/K14</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L20" s="22">
-        <f t="shared" ref="L20" si="2">L5/L14</f>
-        <v>14.999520315841421</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21"/>
-      <c r="B21"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="13" t="e">
-        <f>D6/D15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E21" s="13" t="e">
-        <f>E6/E15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F21" s="13" t="e">
-        <f>F6/F15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G21" s="13" t="e">
-        <f>G6/G15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H21" s="13" t="e">
-        <f>H6/H15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I21" s="13" t="e">
-        <f>I6/I15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J21" s="22" t="e">
-        <f>J6/J15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K21" s="22" t="e">
-        <f>K6/K15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L21" s="22">
-        <f t="shared" ref="L21:L22" si="3">L6/L15</f>
-        <v>11.850265938302314</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22"/>
-      <c r="B22"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="22">
-        <f t="shared" si="3"/>
-        <v>18.640063298590224</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C10" r:id="rId1" xr:uid="{D8C2202D-C06C-4E48-8367-22B62D35A86B}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:L21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" customWidth="1"/>
-    <col min="4" max="9" width="8.85546875" customWidth="1"/>
-    <col min="10" max="12" width="8.85546875" style="18" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2">
-        <v>80</v>
-      </c>
-      <c r="E1" s="2">
-        <v>160</v>
-      </c>
-      <c r="F1" s="2">
-        <v>240</v>
-      </c>
-      <c r="G1" s="2">
-        <v>125</v>
-      </c>
-      <c r="H1" s="2">
-        <v>240</v>
-      </c>
-      <c r="I1" s="2">
-        <v>160</v>
-      </c>
-      <c r="J1" s="15">
-        <v>240</v>
-      </c>
-      <c r="K1" s="15">
-        <v>3200</v>
-      </c>
-      <c r="L1" s="15">
         <v>3600</v>
       </c>
     </row>

</xml_diff>

<commit_message>
experiments to increase the algorithm speed
</commit_message>
<xml_diff>
--- a/python/python_vs_c.xlsx
+++ b/python/python_vs_c.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Library\github\prime\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5930FFA-5EF5-4235-8122-C63EF5DF986D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E937436F-6112-4FDA-9ADC-0783CBD311EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33255" yWindow="2175" windowWidth="15705" windowHeight="13245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="1365" windowWidth="15705" windowHeight="13245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>Python</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>use Feather ESP32-S2 TFT</t>
+  </si>
+  <si>
+    <t>added later</t>
   </si>
 </sst>
 </file>
@@ -127,10 +133,10 @@
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="172" formatCode="0.00000"/>
-    <numFmt numFmtId="173" formatCode="0.000000"/>
-    <numFmt numFmtId="175" formatCode="0.000"/>
-    <numFmt numFmtId="176" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="170" formatCode="#,##0.00000"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -214,7 +220,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -224,6 +230,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -241,7 +253,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -305,10 +317,10 @@
     </xf>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="175" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -324,6 +336,7 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -543,10 +556,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -810,7 +823,9 @@
       <c r="D12" s="29">
         <v>0.01</v>
       </c>
-      <c r="E12" s="31"/>
+      <c r="E12" s="29">
+        <v>0.01</v>
+      </c>
       <c r="F12" s="29">
         <v>0.02</v>
       </c>
@@ -843,7 +858,9 @@
       <c r="D13" s="29">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E13" s="31"/>
+      <c r="E13" s="29">
+        <v>0.3</v>
+      </c>
       <c r="F13" s="29">
         <v>0.43</v>
       </c>
@@ -876,7 +893,9 @@
       <c r="D14" s="29">
         <v>3.29</v>
       </c>
-      <c r="E14" s="31"/>
+      <c r="E14" s="29">
+        <v>7.2</v>
+      </c>
       <c r="F14" s="29">
         <v>10.16</v>
       </c>
@@ -913,7 +932,9 @@
       <c r="D15" s="29">
         <v>82.03</v>
       </c>
-      <c r="E15" s="31"/>
+      <c r="E15" s="29">
+        <v>179.18</v>
+      </c>
       <c r="F15" s="29">
         <v>252.73</v>
       </c>
@@ -954,9 +975,9 @@
         <f t="shared" si="0"/>
         <v>3.60107</v>
       </c>
-      <c r="E18" s="13" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="E18" s="13">
+        <f t="shared" si="0"/>
+        <v>10.9985</v>
       </c>
       <c r="F18" s="13">
         <f t="shared" si="0"/>
@@ -986,9 +1007,9 @@
         <f t="shared" si="0"/>
         <v>4.1713142857142849</v>
       </c>
-      <c r="E19" s="13" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="E19" s="13">
+        <f t="shared" si="0"/>
+        <v>1.7167166666666667</v>
       </c>
       <c r="F19" s="13">
         <f t="shared" si="0"/>
@@ -1018,9 +1039,9 @@
         <f t="shared" si="0"/>
         <v>3.506382978723404</v>
       </c>
-      <c r="E20" s="13" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="E20" s="13">
+        <f t="shared" si="0"/>
+        <v>1.1870833333333335</v>
       </c>
       <c r="F20" s="13">
         <f t="shared" si="0"/>
@@ -1050,9 +1071,9 @@
         <f t="shared" si="0"/>
         <v>3.1871022796537849</v>
       </c>
-      <c r="E21" s="13" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="E21" s="13">
+        <f t="shared" si="0"/>
+        <v>0.94648398258734234</v>
       </c>
       <c r="F21" s="13">
         <f t="shared" si="0"/>
@@ -1086,6 +1107,11 @@
       <c r="I22" s="22">
         <f t="shared" si="4"/>
         <v>18.640063298590224</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1105,7 +1131,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1403,7 +1429,9 @@
       <c r="G11" s="12">
         <v>0.03</v>
       </c>
-      <c r="H11" s="12"/>
+      <c r="H11" s="36">
+        <v>0.01</v>
+      </c>
       <c r="I11" s="12">
         <v>0.02</v>
       </c>
@@ -1432,7 +1460,9 @@
       <c r="G12" s="12">
         <v>0.66</v>
       </c>
-      <c r="H12" s="12"/>
+      <c r="H12" s="36">
+        <v>0.3</v>
+      </c>
       <c r="I12" s="12">
         <v>0.43</v>
       </c>
@@ -1461,7 +1491,9 @@
       <c r="G13" s="12">
         <v>15.82</v>
       </c>
-      <c r="H13" s="12"/>
+      <c r="H13" s="36">
+        <v>7.2</v>
+      </c>
       <c r="I13" s="12">
         <v>10.16</v>
       </c>
@@ -1490,7 +1522,9 @@
       <c r="G14" s="12">
         <v>395.94</v>
       </c>
-      <c r="H14" s="12"/>
+      <c r="H14" s="36">
+        <v>179.18</v>
+      </c>
       <c r="I14" s="12">
         <v>252.78</v>
       </c>
@@ -1499,6 +1533,11 @@
       </c>
       <c r="K14" s="15">
         <v>5.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="3:11" ht="15" x14ac:dyDescent="0.25">
@@ -1518,9 +1557,9 @@
         <f t="shared" si="0"/>
         <v>1.4333333333333333</v>
       </c>
-      <c r="H17" s="13" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="H17" s="13">
+        <f t="shared" si="0"/>
+        <v>13.9</v>
       </c>
       <c r="I17" s="13">
         <f t="shared" si="0"/>
@@ -1553,9 +1592,9 @@
         <f t="shared" si="1"/>
         <v>1.2075757575757575</v>
       </c>
-      <c r="H18" s="13" t="e">
+      <c r="H18" s="13">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>2.5633333333333335</v>
       </c>
       <c r="I18" s="13">
         <f t="shared" si="1"/>
@@ -1588,9 +1627,9 @@
         <f t="shared" si="2"/>
         <v>1.0763590391908975</v>
       </c>
-      <c r="H19" s="13" t="e">
+      <c r="H19" s="13">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1.4275</v>
       </c>
       <c r="I19" s="13">
         <f t="shared" si="2"/>
@@ -1623,9 +1662,9 @@
         <f t="shared" si="3"/>
         <v>1.000911754306208</v>
       </c>
-      <c r="H20" s="13" t="e">
+      <c r="H20" s="13">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1.126649179595937</v>
       </c>
       <c r="I20" s="13">
         <f t="shared" si="3"/>

</xml_diff>